<commit_message>
Consertando problemas com Excel/Onedrive
</commit_message>
<xml_diff>
--- a/regras.xlsx
+++ b/regras.xlsx
@@ -1,24 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artch\OneDrive\ProjetosGit\PycharmProjects\Projeto_Condominio\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8FD881-DA63-4C08-9208-84D5684F3856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E609A51-BDB6-4A07-B3BC-4D7BDCD0CD9F}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="2" sheetId="1" r:id="rId4"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>PalavraChave</t>
   </si>
   <si>
@@ -43,23 +62,50 @@
     <t>Despesa Mensal</t>
   </si>
   <si>
-    <t>...</t>
+    <t>Lucilene Moreira Barbosa</t>
+  </si>
+  <si>
+    <t>MONICA RODRIGUES LIMA VILELA</t>
+  </si>
+  <si>
+    <t>Monica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -68,85 +114,189 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -208,13 +358,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -223,6 +366,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -287,88 +437,103 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8445BEBD-37F3-4B53-A27C-F18D87201428}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.25"/>
-    <col customWidth="1" min="2" max="2" width="35.88"/>
-    <col customWidth="1" min="3" max="3" width="17.25"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>2.0</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>3.0</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>